<commit_message>
Added test.php to test compatability of forecast.ets
</commit_message>
<xml_diff>
--- a/Prototype/PHPSCRIPTS/JASON/ForecastTemplate.xlsx
+++ b/Prototype/PHPSCRIPTS/JASON/ForecastTemplate.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\buzon\Documents\SYSADD2\Forecast-Module-2\Prototype\PHPSCRIPTS\SamanAndrey\Jason\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jade Ericson\Documents\GitHub\Forecast-Module-2\Prototype\PHPSCRIPTS\JASON\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RCK" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -416,11 +416,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,6 +479,18 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
+      <c r="G3" t="e">
+        <f>G2</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H3" t="e">
+        <f>H2</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="I3" t="e">
+        <f>I2</f>
+        <v>#NAME?</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -1423,7 +1435,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2430,7 +2442,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3437,7 +3449,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4444,7 +4456,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5451,7 +5463,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6458,7 +6470,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7465,7 +7477,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8472,7 +8484,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9479,7 +9491,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10486,7 +10498,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11493,7 +11505,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12500,7 +12512,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:I315"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Updated Forecast with Timespan
</commit_message>
<xml_diff>
--- a/Prototype/PHPSCRIPTS/JASON/ForecastTemplate.xlsx
+++ b/Prototype/PHPSCRIPTS/JASON/ForecastTemplate.xlsx
@@ -447,9 +447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I315"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>